<commit_message>
Add A3, A5, A7-A12
</commit_message>
<xml_diff>
--- a/rysiman/evidence.xlsx
+++ b/rysiman/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GON\Rysiman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A4006B-C8D8-49DF-A355-DA63D70A75E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE4C454D-875B-47D9-8397-F5C82AE910AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11760" yWindow="3675" windowWidth="22995" windowHeight="15345" tabRatio="500" firstSheet="1" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="49">
   <si>
     <t>TeamName</t>
   </si>
@@ -87,15 +87,6 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>nft id</t>
-  </si>
-  <si>
-    <t>tx hash on dest chain</t>
-  </si>
-  <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
     <t>tx hash on that chain</t>
   </si>
   <si>
@@ -166,13 +157,52 @@
   </si>
   <si>
     <t>5CE6A349A042E20E4F4441924679D80FC444271241BCE0B280EBDA57D7353EB3</t>
+  </si>
+  <si>
+    <t>14068E1916518AC76C9FB4F6A5F99FE9810C527DECC142B19924D88954ED17E5</t>
+  </si>
+  <si>
+    <t>rysigon44</t>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>E4CCD456D8E1124C5E4B063A9983731F17ECAA509B7648D824357D49999CE496</t>
+  </si>
+  <si>
+    <t>rysigon04</t>
+  </si>
+  <si>
+    <t>03A69A159F1DAC5F0490027D0F096EB6E8431A60498D532993144440ED327AB8</t>
+  </si>
+  <si>
+    <t>75D8ECB14016DD5D89CE8EA56ACDB311228C5F8C848B36C808B64EC8F28B6843</t>
+  </si>
+  <si>
+    <t>stars1mgcpkhw4yx4hhygtzt99wlj2d8el23g29g8x0f2zf754a0clcr0q4exy9m</t>
+  </si>
+  <si>
+    <t>rysigon07</t>
+  </si>
+  <si>
+    <t>rysigon12</t>
+  </si>
+  <si>
+    <t>rysigon10</t>
+  </si>
+  <si>
+    <t>rysigon09</t>
+  </si>
+  <si>
+    <t>rysigon08</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -189,13 +219,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -248,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -263,7 +286,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -692,28 +714,28 @@
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="G2" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -726,7 +748,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -744,10 +768,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -760,7 +784,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -778,10 +804,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -794,7 +820,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -812,10 +840,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -828,7 +856,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -846,10 +876,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -880,20 +910,20 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -924,20 +954,20 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -968,20 +998,20 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1012,20 +1042,20 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1056,20 +1086,20 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1100,20 +1130,20 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1126,7 +1156,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1145,10 +1175,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1179,20 +1209,20 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1223,20 +1253,20 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1263,12 +1293,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1295,12 +1325,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1327,12 +1357,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1359,12 +1389,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1375,10 +1405,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C3"/>
+      <selection activeCell="A4" sqref="A4:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1400,29 +1430,51 @@
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1431,7 +1483,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,10 +1508,18 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1498,16 +1558,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1521,7 +1581,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1547,15 +1607,17 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="6"/>
+        <v>42</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1595,16 +1657,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1617,7 +1679,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1635,10 +1699,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1651,7 +1715,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1669,10 +1735,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>